<commit_message>
PTH increase by 50%
</commit_message>
<xml_diff>
--- a/16-May-2023_model_results.xlsx
+++ b/16-May-2023_model_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofwaterloo-my.sharepoint.com/personal/mstadt_uwaterloo_ca/Documents/Layton Lab Research/calcium/Manuscript_CaReg_FemPregLact/code/CaReg_FemPregLact/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_714DB1978EFED742421EF3677D7CBDB740334C09" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60EC345E-1CAF-4F1A-A47A-4902A46F20F1}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_714DB1978EFED742421EF3677D7CBDB740334C09" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E9EBE1E5-4EA4-48B5-AF89-B16931B65CF4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -627,8 +627,8 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F54" sqref="F54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>